<commit_message>
Additional patient columns in AU Core Sample Data.xlsx
</commit_message>
<xml_diff>
--- a/Sparked.Csv2FhirMapping/TestData/AU Core Sample Data.xlsx
+++ b/Sparked.Csv2FhirMapping/TestData/AU Core Sample Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau.sharepoint.com/sites/DoHACCSIROdigitalhealthcollaborationspace/Shared Documents/AU Core TDG/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3110" documentId="8_{9B812D32-04E3-4A00-9431-8964624A4549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59BE6AFC-8E9C-410E-95B4-2BB72488FAF8}"/>
+  <xr:revisionPtr revIDLastSave="3166" documentId="8_{9B812D32-04E3-4A00-9431-8964624A4549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DBBBE9-265F-413B-9287-8A1C61FC250F}"/>
   <bookViews>
     <workbookView xWindow="13965" yWindow="165" windowWidth="23880" windowHeight="20565" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="1170">
   <si>
     <t>id</t>
   </si>
@@ -3463,12 +3463,6 @@
     <t>Medical Record Number</t>
   </si>
   <si>
-    <t>identifier_ihiStatus_code</t>
-  </si>
-  <si>
-    <t>identifier_ihiRecordStatus_code</t>
-  </si>
-  <si>
     <t>identifier3_type_display</t>
   </si>
   <si>
@@ -3481,16 +3475,70 @@
     <t>name1_text</t>
   </si>
   <si>
-    <t>telecom_system</t>
-  </si>
-  <si>
-    <t>telecom_use</t>
-  </si>
-  <si>
-    <t>telecom_value</t>
-  </si>
-  <si>
     <t>birthDate_accurancyIndicator_code</t>
+  </si>
+  <si>
+    <t>identifier1_ihiRecordStatus_code</t>
+  </si>
+  <si>
+    <t>identifier1_ihiStatus_code</t>
+  </si>
+  <si>
+    <t>name2_use</t>
+  </si>
+  <si>
+    <t>name2_text</t>
+  </si>
+  <si>
+    <t>name2_family</t>
+  </si>
+  <si>
+    <t>name2_given1</t>
+  </si>
+  <si>
+    <t>name2_prefix</t>
+  </si>
+  <si>
+    <t>name1_given2</t>
+  </si>
+  <si>
+    <t>name2_given2</t>
+  </si>
+  <si>
+    <t>telecom3_system</t>
+  </si>
+  <si>
+    <t>telecom3_use</t>
+  </si>
+  <si>
+    <t>telecom3_value</t>
+  </si>
+  <si>
+    <t>Day, month and year are accurate</t>
+  </si>
+  <si>
+    <t>birthDate_accurancyIndicator_display</t>
+  </si>
+  <si>
+    <t>address2_use</t>
+  </si>
+  <si>
+    <t>address2_line1</t>
+  </si>
+  <si>
+    <t>address2_line2</t>
+  </si>
+  <si>
+    <t>address2_city</t>
+  </si>
+  <si>
+    <t>address2_state</t>
+  </si>
+  <si>
+    <t>address2_postalCode</t>
+  </si>
+  <si>
+    <t>address2_country</t>
   </si>
 </sst>
 </file>
@@ -4353,10 +4401,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY7"/>
+  <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="BF1" sqref="BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4378,38 +4429,52 @@
     <col min="15" max="15" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="19.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.28515625" style="1" customWidth="1"/>
     <col min="23" max="23" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="21" style="1" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21" style="1" customWidth="1"/>
     <col min="27" max="27" width="19.42578125" style="1" customWidth="1"/>
     <col min="28" max="28" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="1"/>
+    <col min="30" max="30" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.42578125" style="1" customWidth="1"/>
-    <col min="43" max="43" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14" style="1" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="41" width="13.42578125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="27.42578125" style="1" customWidth="1"/>
+    <col min="57" max="57" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="22.140625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="69" width="22.140625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4432,10 +4497,10 @@
         <v>95</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1144</v>
+        <v>1150</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>1145</v>
+        <v>1149</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>1</v>
@@ -4483,10 +4548,10 @@
         <v>1133</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>1135</v>
@@ -4501,7 +4566,7 @@
         <v>7</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="AF1" s="3" t="s">
         <v>4</v>
@@ -4510,10 +4575,10 @@
         <v>5</v>
       </c>
       <c r="AH1" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>1150</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>1151</v>
@@ -4522,49 +4587,115 @@
         <v>1152</v>
       </c>
       <c r="AL1" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>1159</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="AY1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" s="3" t="s">
-        <v>1153</v>
-      </c>
-      <c r="AP1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="BD1" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="BG1" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="BR1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -4590,7 +4721,7 @@
         <v>6951449677</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>20</v>
@@ -4601,53 +4732,53 @@
       <c r="AG2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AT2" s="1">
+      <c r="BI2" s="1">
         <v>4112</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -4675,17 +4806,17 @@
       <c r="AG3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AY3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="BA3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -4716,44 +4847,44 @@
       <c r="AG4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AY4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AZ4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AP4" s="1" t="s">
+      <c r="BD4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="BE4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="BG4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="BH4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AT4" s="1">
+      <c r="BI4" s="1">
         <v>2148</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="BJ4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -4793,35 +4924,35 @@
       <c r="AG5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AI5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AY5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AZ5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AP5" s="1" t="s">
+      <c r="BD5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="BE5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="BG5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="BH5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AT5" s="2" t="s">
+      <c r="BI5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AU5" s="1" t="s">
+      <c r="BJ5" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
@@ -4858,17 +4989,17 @@
       <c r="AG6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AY6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AZ6" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -4945,46 +5076,49 @@
       <c r="AG7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AY7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM7" s="1" t="s">
+      <c r="AZ7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AO7" s="1" t="s">
+      <c r="BB7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AP7" s="1" t="s">
+      <c r="BC7" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="BD7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ7" s="1" t="s">
+      <c r="BE7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AR7" s="1" t="s">
+      <c r="BG7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AS7" s="1" t="s">
+      <c r="BH7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AT7" s="1">
+      <c r="BI7" s="1">
         <v>2148</v>
       </c>
-      <c r="AU7" s="1" t="s">
+      <c r="BJ7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AV7" s="1" t="s">
+      <c r="BR7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AW7" s="1" t="s">
+      <c r="BS7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AX7" s="1" t="s">
+      <c r="BT7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AY7" s="1" t="s">
+      <c r="BU7" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -12760,12 +12894,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E0EA801C84535243AB84D3C1248501C3" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58d70cd10eec94b82c5d8662dcfcbecd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c6a070e6-a3c1-408c-90db-f61ae761556c" xmlns:ns3="5cf10198-f610-4117-95cd-801043105cf8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb249e35e779f88a3ab4217bfb2f2887" ns2:_="" ns3:_="">
     <xsd:import namespace="c6a070e6-a3c1-408c-90db-f61ae761556c"/>
@@ -12948,6 +13076,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31331A8-428E-4E89-871C-985431B13279}">
   <ds:schemaRefs>
@@ -12957,23 +13091,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C03F3D70-B048-47AE-A282-C22FCB8FC77C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5cf10198-f610-4117-95cd-801043105cf8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c6a070e6-a3c1-408c-90db-f61ae761556c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442002CC-009F-41F7-AA3E-49A9BC650F93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12990,4 +13107,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C03F3D70-B048-47AE-A282-C22FCB8FC77C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="5cf10198-f610-4117-95cd-801043105cf8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c6a070e6-a3c1-408c-90db-f61ae761556c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>